<commit_message>
får ikke til sortering av dagsverk
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
   <si>
     <t>Uke</t>
   </si>
@@ -41,127 +41,178 @@
     <t>Søndag</t>
   </si>
   <si>
-    <t>6:00 - 14:00 - 9324-X</t>
-  </si>
-  <si>
-    <t>TT</t>
-  </si>
-  <si>
-    <t>XX</t>
-  </si>
-  <si>
-    <t>14:36 - 22:23</t>
-  </si>
-  <si>
-    <t>8:01 - 17:29</t>
-  </si>
-  <si>
-    <t>OO</t>
-  </si>
-  <si>
-    <t>23:37 - 7:31</t>
-  </si>
-  <si>
-    <t>13:31 - 21:23</t>
-  </si>
-  <si>
-    <t>6:00 - 14:00</t>
-  </si>
-  <si>
-    <t>15:00 - 23:00</t>
-  </si>
-  <si>
-    <t>21:39 - 5:45</t>
-  </si>
-  <si>
-    <t>14:00 - 22:00</t>
-  </si>
-  <si>
-    <t>9:40 - 19:06</t>
-  </si>
-  <si>
-    <t>5:30 - 15:00</t>
-  </si>
-  <si>
-    <t>7:13 - 15:01</t>
-  </si>
-  <si>
-    <t>14:01 - 21:42</t>
-  </si>
-  <si>
-    <t>5:00 - 13:00</t>
-  </si>
-  <si>
-    <t>7:17 - 15:17</t>
-  </si>
-  <si>
-    <t>6:00 - 15:00</t>
-  </si>
-  <si>
-    <t>16:07 - 22:38</t>
-  </si>
-  <si>
-    <t>23:00 - 7:00</t>
-  </si>
-  <si>
-    <t>7:35 - 15:47</t>
-  </si>
-  <si>
-    <t>13:00 - 21:00</t>
-  </si>
-  <si>
-    <t>23:45 - 7:36</t>
-  </si>
-  <si>
-    <t>7:43 - 16:20</t>
-  </si>
-  <si>
-    <t>15:00 - 23:00 - 9309</t>
-  </si>
-  <si>
-    <t>15:08 - 22:26</t>
-  </si>
-  <si>
-    <t>23:23 - 6:28</t>
-  </si>
-  <si>
-    <t>6:00 - 16:00</t>
-  </si>
-  <si>
-    <t>21:23 - 7:28</t>
-  </si>
-  <si>
-    <t>14:45 - 22:56</t>
-  </si>
-  <si>
-    <t>22:00 - 6:00</t>
-  </si>
-  <si>
-    <t>6:33 - 13:13</t>
-  </si>
-  <si>
-    <t>7:00 - 16:00</t>
-  </si>
-  <si>
-    <t>15:12 - 22:20</t>
-  </si>
-  <si>
-    <t>7:21 - 14:33</t>
-  </si>
-  <si>
-    <t>7:00 - 15:00</t>
-  </si>
-  <si>
-    <t>9:41 - 20:08</t>
-  </si>
-  <si>
-    <t>13:28 - 22:38</t>
-  </si>
-  <si>
-    <t>10:35 - 19:38</t>
-  </si>
-  <si>
-    <t>15:18 - 22:28</t>
+    <t>6:00 - 14:00 9324-X</t>
+  </si>
+  <si>
+    <t>TT 5018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XX </t>
+  </si>
+  <si>
+    <t>14:36 - 22:23 3006</t>
+  </si>
+  <si>
+    <t>8:01 - 17:29 9303</t>
+  </si>
+  <si>
+    <t>OO 9309</t>
+  </si>
+  <si>
+    <t>23:37 - 7:31 1576</t>
+  </si>
+  <si>
+    <t>13:31 - 21:23 9327-X</t>
+  </si>
+  <si>
+    <t>OO 1429</t>
+  </si>
+  <si>
+    <t>6:00 - 14:00 905301500</t>
+  </si>
+  <si>
+    <t>15:00 - 23:00 9308</t>
+  </si>
+  <si>
+    <t>8:01 - 17:29 5014</t>
+  </si>
+  <si>
+    <t>21:39 - 5:45 1567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:00 - 22:00 </t>
+  </si>
+  <si>
+    <t>9:40 - 19:06 5005-73</t>
+  </si>
+  <si>
+    <t>5:30 - 15:00 9301</t>
+  </si>
+  <si>
+    <t>14:00 - 22:00 9329-X</t>
+  </si>
+  <si>
+    <t>7:13 - 15:01 1424-Mod1</t>
+  </si>
+  <si>
+    <t>TT 9906001500-H</t>
+  </si>
+  <si>
+    <t>14:01 - 21:42 1235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:00 - 13:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:00 - 23:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:17 - 15:17 </t>
+  </si>
+  <si>
+    <t>OO 1607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:00 - 15:00 </t>
+  </si>
+  <si>
+    <t>16:07 - 22:38 9306</t>
+  </si>
+  <si>
+    <t>23:00 - 7:00 9312</t>
+  </si>
+  <si>
+    <t>7:35 - 15:47 1705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:00 - 21:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OO </t>
+  </si>
+  <si>
+    <t>23:45 - 7:36 1775</t>
+  </si>
+  <si>
+    <t>7:43 - 16:20 3008</t>
+  </si>
+  <si>
+    <t>15:00 - 23:00 9309</t>
+  </si>
+  <si>
+    <t>15:08 - 22:26 5005-73</t>
+  </si>
+  <si>
+    <t>OO 906001600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:31 - 21:23 </t>
+  </si>
+  <si>
+    <t>23:23 - 6:28 3119</t>
+  </si>
+  <si>
+    <t>14:01 - 21:42 1447</t>
+  </si>
+  <si>
+    <t>6:00 - 16:00 9322-X</t>
+  </si>
+  <si>
+    <t>21:23 - 7:28 3109</t>
+  </si>
+  <si>
+    <t>14:45 - 22:56 9330-X</t>
+  </si>
+  <si>
+    <t>22:00 - 6:00 9331-X</t>
+  </si>
+  <si>
+    <t>6:00 - 16:00 5002</t>
+  </si>
+  <si>
+    <t>XX 9323-X</t>
+  </si>
+  <si>
+    <t>6:33 - 13:13 1458-Mod1</t>
+  </si>
+  <si>
+    <t>TT 3101</t>
+  </si>
+  <si>
+    <t>OO 9323-X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT </t>
+  </si>
+  <si>
+    <t>6:00 - 14:00 9305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:00 - 16:00 </t>
+  </si>
+  <si>
+    <t>15:12 - 22:20 3020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:21 - 14:33 </t>
+  </si>
+  <si>
+    <t>6:00 - 14:00 3031</t>
+  </si>
+  <si>
+    <t>7:00 - 15:00 3134</t>
+  </si>
+  <si>
+    <t>9:41 - 20:08 3132</t>
+  </si>
+  <si>
+    <t>13:28 - 22:38 5004</t>
+  </si>
+  <si>
+    <t>10:35 - 19:38 3006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:18 - 22:28 </t>
   </si>
 </sst>
 </file>
@@ -620,19 +671,19 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32" customHeight="1">
@@ -646,19 +697,19 @@
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="32" customHeight="1">
@@ -672,19 +723,19 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32" customHeight="1">
@@ -696,19 +747,19 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="32" customHeight="1">
@@ -722,17 +773,17 @@
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="32" customHeight="1">
@@ -746,19 +797,19 @@
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +830,7 @@
       <formula>(B2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
-      <formula>(B2="XX")OR (B2="OO")OR (B2="TT")</formula>
+      <formula>(B2="XX ")OR (B2="OO ")OR (B2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
@@ -799,7 +850,7 @@
       <formula>(B3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="12">
-      <formula>(B3="XX")OR (B3="OO")OR (B3="TT")</formula>
+      <formula>(B3="XX ")OR (B3="OO ")OR (B3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
@@ -819,7 +870,7 @@
       <formula>(B4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="18">
-      <formula>(B4="XX")OR (B4="OO")OR (B4="TT")</formula>
+      <formula>(B4="XX ")OR (B4="OO ")OR (B4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
@@ -839,7 +890,7 @@
       <formula>(B5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="24">
-      <formula>(B5="XX")OR (B5="OO")OR (B5="TT")</formula>
+      <formula>(B5="XX ")OR (B5="OO ")OR (B5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
@@ -859,7 +910,7 @@
       <formula>(B6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="30">
-      <formula>(B6="XX")OR (B6="OO")OR (B6="TT")</formula>
+      <formula>(B6="XX ")OR (B6="OO ")OR (B6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
@@ -879,7 +930,7 @@
       <formula>(B7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="36">
-      <formula>(B7="XX")OR (B7="OO")OR (B7="TT")</formula>
+      <formula>(B7="XX ")OR (B7="OO ")OR (B7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
@@ -899,7 +950,7 @@
       <formula>(C2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="42">
-      <formula>(C2="XX")OR (C2="OO")OR (C2="TT")</formula>
+      <formula>(C2="XX ")OR (C2="OO ")OR (C2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
@@ -919,7 +970,7 @@
       <formula>(C3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="48">
-      <formula>(C3="XX")OR (C3="OO")OR (C3="TT")</formula>
+      <formula>(C3="XX ")OR (C3="OO ")OR (C3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
@@ -939,7 +990,7 @@
       <formula>(C4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="54">
-      <formula>(C4="XX")OR (C4="OO")OR (C4="TT")</formula>
+      <formula>(C4="XX ")OR (C4="OO ")OR (C4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
@@ -959,7 +1010,7 @@
       <formula>(C5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="60">
-      <formula>(C5="XX")OR (C5="OO")OR (C5="TT")</formula>
+      <formula>(C5="XX ")OR (C5="OO ")OR (C5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
@@ -979,7 +1030,7 @@
       <formula>(C6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="66">
-      <formula>(C6="XX")OR (C6="OO")OR (C6="TT")</formula>
+      <formula>(C6="XX ")OR (C6="OO ")OR (C6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
@@ -999,7 +1050,7 @@
       <formula>(C7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="72">
-      <formula>(C7="XX")OR (C7="OO")OR (C7="TT")</formula>
+      <formula>(C7="XX ")OR (C7="OO ")OR (C7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
@@ -1019,7 +1070,7 @@
       <formula>(D2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="78">
-      <formula>(D2="XX")OR (D2="OO")OR (D2="TT")</formula>
+      <formula>(D2="XX ")OR (D2="OO ")OR (D2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
@@ -1039,7 +1090,7 @@
       <formula>(D3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="84">
-      <formula>(D3="XX")OR (D3="OO")OR (D3="TT")</formula>
+      <formula>(D3="XX ")OR (D3="OO ")OR (D3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
@@ -1059,7 +1110,7 @@
       <formula>(D4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="90">
-      <formula>(D4="XX")OR (D4="OO")OR (D4="TT")</formula>
+      <formula>(D4="XX ")OR (D4="OO ")OR (D4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
@@ -1079,7 +1130,7 @@
       <formula>(D5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="96">
-      <formula>(D5="XX")OR (D5="OO")OR (D5="TT")</formula>
+      <formula>(D5="XX ")OR (D5="OO ")OR (D5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
@@ -1099,7 +1150,7 @@
       <formula>(D6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="102">
-      <formula>(D6="XX")OR (D6="OO")OR (D6="TT")</formula>
+      <formula>(D6="XX ")OR (D6="OO ")OR (D6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
@@ -1119,7 +1170,7 @@
       <formula>(D7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="108">
-      <formula>(D7="XX")OR (D7="OO")OR (D7="TT")</formula>
+      <formula>(D7="XX ")OR (D7="OO ")OR (D7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
@@ -1139,7 +1190,7 @@
       <formula>(E2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="114">
-      <formula>(E2="XX")OR (E2="OO")OR (E2="TT")</formula>
+      <formula>(E2="XX ")OR (E2="OO ")OR (E2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
@@ -1159,7 +1210,7 @@
       <formula>(E3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="120">
-      <formula>(E3="XX")OR (E3="OO")OR (E3="TT")</formula>
+      <formula>(E3="XX ")OR (E3="OO ")OR (E3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
@@ -1179,7 +1230,7 @@
       <formula>(E4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="126">
-      <formula>(E4="XX")OR (E4="OO")OR (E4="TT")</formula>
+      <formula>(E4="XX ")OR (E4="OO ")OR (E4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
@@ -1199,7 +1250,7 @@
       <formula>(E5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="132">
-      <formula>(E5="XX")OR (E5="OO")OR (E5="TT")</formula>
+      <formula>(E5="XX ")OR (E5="OO ")OR (E5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
@@ -1219,7 +1270,7 @@
       <formula>(E6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="138">
-      <formula>(E6="XX")OR (E6="OO")OR (E6="TT")</formula>
+      <formula>(E6="XX ")OR (E6="OO ")OR (E6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
@@ -1239,7 +1290,7 @@
       <formula>(E7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="144">
-      <formula>(E7="XX")OR (E7="OO")OR (E7="TT")</formula>
+      <formula>(E7="XX ")OR (E7="OO ")OR (E7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
@@ -1259,7 +1310,7 @@
       <formula>(F2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="150">
-      <formula>(F2="XX")OR (F2="OO")OR (F2="TT")</formula>
+      <formula>(F2="XX ")OR (F2="OO ")OR (F2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
@@ -1279,7 +1330,7 @@
       <formula>(F3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="156">
-      <formula>(F3="XX")OR (F3="OO")OR (F3="TT")</formula>
+      <formula>(F3="XX ")OR (F3="OO ")OR (F3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
@@ -1299,7 +1350,7 @@
       <formula>(F4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="162">
-      <formula>(F4="XX")OR (F4="OO")OR (F4="TT")</formula>
+      <formula>(F4="XX ")OR (F4="OO ")OR (F4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
@@ -1319,7 +1370,7 @@
       <formula>(F5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="168">
-      <formula>(F5="XX")OR (F5="OO")OR (F5="TT")</formula>
+      <formula>(F5="XX ")OR (F5="OO ")OR (F5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
@@ -1339,7 +1390,7 @@
       <formula>(F6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="174">
-      <formula>(F6="XX")OR (F6="OO")OR (F6="TT")</formula>
+      <formula>(F6="XX ")OR (F6="OO ")OR (F6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
@@ -1359,7 +1410,7 @@
       <formula>(F7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="180">
-      <formula>(F7="XX")OR (F7="OO")OR (F7="TT")</formula>
+      <formula>(F7="XX ")OR (F7="OO ")OR (F7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
@@ -1379,7 +1430,7 @@
       <formula>(G2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="186">
-      <formula>(G2="XX")OR (G2="OO")OR (G2="TT")</formula>
+      <formula>(G2="XX ")OR (G2="OO ")OR (G2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
@@ -1399,7 +1450,7 @@
       <formula>(G3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="192">
-      <formula>(G3="XX")OR (G3="OO")OR (G3="TT")</formula>
+      <formula>(G3="XX ")OR (G3="OO ")OR (G3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
@@ -1419,7 +1470,7 @@
       <formula>(G4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="198">
-      <formula>(G4="XX")OR (G4="OO")OR (G4="TT")</formula>
+      <formula>(G4="XX ")OR (G4="OO ")OR (G4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
@@ -1439,7 +1490,7 @@
       <formula>(G5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="204">
-      <formula>(G5="XX")OR (G5="OO")OR (G5="TT")</formula>
+      <formula>(G5="XX ")OR (G5="OO ")OR (G5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
@@ -1459,7 +1510,7 @@
       <formula>(G6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="210">
-      <formula>(G6="XX")OR (G6="OO")OR (G6="TT")</formula>
+      <formula>(G6="XX ")OR (G6="OO ")OR (G6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
@@ -1479,7 +1530,7 @@
       <formula>(G7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="216">
-      <formula>(G7="XX")OR (G7="OO")OR (G7="TT")</formula>
+      <formula>(G7="XX ")OR (G7="OO ")OR (G7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
@@ -1499,7 +1550,7 @@
       <formula>(H2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="222">
-      <formula>(H2="XX")OR (H2="OO")OR (H2="TT")</formula>
+      <formula>(H2="XX ")OR (H2="OO ")OR (H2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
@@ -1519,7 +1570,7 @@
       <formula>(H3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="228">
-      <formula>(H3="XX")OR (H3="OO")OR (H3="TT")</formula>
+      <formula>(H3="XX ")OR (H3="OO ")OR (H3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
@@ -1539,7 +1590,7 @@
       <formula>(H4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="234">
-      <formula>(H4="XX")OR (H4="OO")OR (H4="TT")</formula>
+      <formula>(H4="XX ")OR (H4="OO ")OR (H4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
@@ -1559,7 +1610,7 @@
       <formula>(H5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="240">
-      <formula>(H5="XX")OR (H5="OO")OR (H5="TT")</formula>
+      <formula>(H5="XX ")OR (H5="OO ")OR (H5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
@@ -1579,7 +1630,7 @@
       <formula>(H6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="246">
-      <formula>(H6="XX")OR (H6="OO")OR (H6="TT")</formula>
+      <formula>(H6="XX ")OR (H6="OO ")OR (H6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
@@ -1599,7 +1650,7 @@
       <formula>(H7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="252">
-      <formula>(H7="XX")OR (H7="OO")OR (H7="TT")</formula>
+      <formula>(H7="XX ")OR (H7="OO ")OR (H7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1649,23 +1700,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32" customHeight="1">
@@ -1673,25 +1724,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="32" customHeight="1">
@@ -1699,25 +1750,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32" customHeight="1">
@@ -1725,23 +1776,23 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="32" customHeight="1">
@@ -1752,22 +1803,22 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="32" customHeight="1">
@@ -1775,23 +1826,23 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1863,7 @@
       <formula>(B2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
-      <formula>(B2="XX")OR (B2="OO")OR (B2="TT")</formula>
+      <formula>(B2="XX ")OR (B2="OO ")OR (B2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
@@ -1832,7 +1883,7 @@
       <formula>(B3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="12">
-      <formula>(B3="XX")OR (B3="OO")OR (B3="TT")</formula>
+      <formula>(B3="XX ")OR (B3="OO ")OR (B3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
@@ -1852,7 +1903,7 @@
       <formula>(B4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="18">
-      <formula>(B4="XX")OR (B4="OO")OR (B4="TT")</formula>
+      <formula>(B4="XX ")OR (B4="OO ")OR (B4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
@@ -1872,7 +1923,7 @@
       <formula>(B5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="24">
-      <formula>(B5="XX")OR (B5="OO")OR (B5="TT")</formula>
+      <formula>(B5="XX ")OR (B5="OO ")OR (B5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
@@ -1892,7 +1943,7 @@
       <formula>(B6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="30">
-      <formula>(B6="XX")OR (B6="OO")OR (B6="TT")</formula>
+      <formula>(B6="XX ")OR (B6="OO ")OR (B6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
@@ -1912,7 +1963,7 @@
       <formula>(B7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="36">
-      <formula>(B7="XX")OR (B7="OO")OR (B7="TT")</formula>
+      <formula>(B7="XX ")OR (B7="OO ")OR (B7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
@@ -1932,7 +1983,7 @@
       <formula>(C2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="42">
-      <formula>(C2="XX")OR (C2="OO")OR (C2="TT")</formula>
+      <formula>(C2="XX ")OR (C2="OO ")OR (C2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
@@ -1952,7 +2003,7 @@
       <formula>(C3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="48">
-      <formula>(C3="XX")OR (C3="OO")OR (C3="TT")</formula>
+      <formula>(C3="XX ")OR (C3="OO ")OR (C3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
@@ -1972,7 +2023,7 @@
       <formula>(C4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="54">
-      <formula>(C4="XX")OR (C4="OO")OR (C4="TT")</formula>
+      <formula>(C4="XX ")OR (C4="OO ")OR (C4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
@@ -1992,7 +2043,7 @@
       <formula>(C5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="60">
-      <formula>(C5="XX")OR (C5="OO")OR (C5="TT")</formula>
+      <formula>(C5="XX ")OR (C5="OO ")OR (C5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
@@ -2012,7 +2063,7 @@
       <formula>(C6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="66">
-      <formula>(C6="XX")OR (C6="OO")OR (C6="TT")</formula>
+      <formula>(C6="XX ")OR (C6="OO ")OR (C6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
@@ -2032,7 +2083,7 @@
       <formula>(C7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="72">
-      <formula>(C7="XX")OR (C7="OO")OR (C7="TT")</formula>
+      <formula>(C7="XX ")OR (C7="OO ")OR (C7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
@@ -2052,7 +2103,7 @@
       <formula>(D2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="78">
-      <formula>(D2="XX")OR (D2="OO")OR (D2="TT")</formula>
+      <formula>(D2="XX ")OR (D2="OO ")OR (D2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
@@ -2072,7 +2123,7 @@
       <formula>(D3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="84">
-      <formula>(D3="XX")OR (D3="OO")OR (D3="TT")</formula>
+      <formula>(D3="XX ")OR (D3="OO ")OR (D3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
@@ -2092,7 +2143,7 @@
       <formula>(D4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="90">
-      <formula>(D4="XX")OR (D4="OO")OR (D4="TT")</formula>
+      <formula>(D4="XX ")OR (D4="OO ")OR (D4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
@@ -2112,7 +2163,7 @@
       <formula>(D5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="96">
-      <formula>(D5="XX")OR (D5="OO")OR (D5="TT")</formula>
+      <formula>(D5="XX ")OR (D5="OO ")OR (D5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
@@ -2132,7 +2183,7 @@
       <formula>(D6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="102">
-      <formula>(D6="XX")OR (D6="OO")OR (D6="TT")</formula>
+      <formula>(D6="XX ")OR (D6="OO ")OR (D6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
@@ -2152,7 +2203,7 @@
       <formula>(D7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="108">
-      <formula>(D7="XX")OR (D7="OO")OR (D7="TT")</formula>
+      <formula>(D7="XX ")OR (D7="OO ")OR (D7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
@@ -2172,7 +2223,7 @@
       <formula>(E2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="114">
-      <formula>(E2="XX")OR (E2="OO")OR (E2="TT")</formula>
+      <formula>(E2="XX ")OR (E2="OO ")OR (E2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
@@ -2192,7 +2243,7 @@
       <formula>(E3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="120">
-      <formula>(E3="XX")OR (E3="OO")OR (E3="TT")</formula>
+      <formula>(E3="XX ")OR (E3="OO ")OR (E3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
@@ -2212,7 +2263,7 @@
       <formula>(E4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="126">
-      <formula>(E4="XX")OR (E4="OO")OR (E4="TT")</formula>
+      <formula>(E4="XX ")OR (E4="OO ")OR (E4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
@@ -2232,7 +2283,7 @@
       <formula>(E5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="132">
-      <formula>(E5="XX")OR (E5="OO")OR (E5="TT")</formula>
+      <formula>(E5="XX ")OR (E5="OO ")OR (E5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
@@ -2252,7 +2303,7 @@
       <formula>(E6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="138">
-      <formula>(E6="XX")OR (E6="OO")OR (E6="TT")</formula>
+      <formula>(E6="XX ")OR (E6="OO ")OR (E6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
@@ -2272,7 +2323,7 @@
       <formula>(E7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="144">
-      <formula>(E7="XX")OR (E7="OO")OR (E7="TT")</formula>
+      <formula>(E7="XX ")OR (E7="OO ")OR (E7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
@@ -2292,7 +2343,7 @@
       <formula>(F2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="150">
-      <formula>(F2="XX")OR (F2="OO")OR (F2="TT")</formula>
+      <formula>(F2="XX ")OR (F2="OO ")OR (F2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
@@ -2312,7 +2363,7 @@
       <formula>(F3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="156">
-      <formula>(F3="XX")OR (F3="OO")OR (F3="TT")</formula>
+      <formula>(F3="XX ")OR (F3="OO ")OR (F3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
@@ -2332,7 +2383,7 @@
       <formula>(F4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="162">
-      <formula>(F4="XX")OR (F4="OO")OR (F4="TT")</formula>
+      <formula>(F4="XX ")OR (F4="OO ")OR (F4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
@@ -2352,7 +2403,7 @@
       <formula>(F5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="168">
-      <formula>(F5="XX")OR (F5="OO")OR (F5="TT")</formula>
+      <formula>(F5="XX ")OR (F5="OO ")OR (F5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
@@ -2372,7 +2423,7 @@
       <formula>(F6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="174">
-      <formula>(F6="XX")OR (F6="OO")OR (F6="TT")</formula>
+      <formula>(F6="XX ")OR (F6="OO ")OR (F6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
@@ -2392,7 +2443,7 @@
       <formula>(F7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="180">
-      <formula>(F7="XX")OR (F7="OO")OR (F7="TT")</formula>
+      <formula>(F7="XX ")OR (F7="OO ")OR (F7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
@@ -2412,7 +2463,7 @@
       <formula>(G2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="186">
-      <formula>(G2="XX")OR (G2="OO")OR (G2="TT")</formula>
+      <formula>(G2="XX ")OR (G2="OO ")OR (G2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
@@ -2432,7 +2483,7 @@
       <formula>(G3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="192">
-      <formula>(G3="XX")OR (G3="OO")OR (G3="TT")</formula>
+      <formula>(G3="XX ")OR (G3="OO ")OR (G3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
@@ -2452,7 +2503,7 @@
       <formula>(G4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="198">
-      <formula>(G4="XX")OR (G4="OO")OR (G4="TT")</formula>
+      <formula>(G4="XX ")OR (G4="OO ")OR (G4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
@@ -2472,7 +2523,7 @@
       <formula>(G5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="204">
-      <formula>(G5="XX")OR (G5="OO")OR (G5="TT")</formula>
+      <formula>(G5="XX ")OR (G5="OO ")OR (G5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
@@ -2492,7 +2543,7 @@
       <formula>(G6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="210">
-      <formula>(G6="XX")OR (G6="OO")OR (G6="TT")</formula>
+      <formula>(G6="XX ")OR (G6="OO ")OR (G6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
@@ -2512,7 +2563,7 @@
       <formula>(G7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="216">
-      <formula>(G7="XX")OR (G7="OO")OR (G7="TT")</formula>
+      <formula>(G7="XX ")OR (G7="OO ")OR (G7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
@@ -2532,7 +2583,7 @@
       <formula>(H2="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="222">
-      <formula>(H2="XX")OR (H2="OO")OR (H2="TT")</formula>
+      <formula>(H2="XX ")OR (H2="OO ")OR (H2="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
@@ -2552,7 +2603,7 @@
       <formula>(H3="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="228">
-      <formula>(H3="XX")OR (H3="OO")OR (H3="TT")</formula>
+      <formula>(H3="XX ")OR (H3="OO ")OR (H3="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
@@ -2572,7 +2623,7 @@
       <formula>(H4="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="234">
-      <formula>(H4="XX")OR (H4="OO")OR (H4="TT")</formula>
+      <formula>(H4="XX ")OR (H4="OO ")OR (H4="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
@@ -2592,7 +2643,7 @@
       <formula>(H5="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="240">
-      <formula>(H5="XX")OR (H5="OO")OR (H5="TT")</formula>
+      <formula>(H5="XX ")OR (H5="OO ")OR (H5="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
@@ -2612,7 +2663,7 @@
       <formula>(H6="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="246">
-      <formula>(H6="XX")OR (H6="OO")OR (H6="TT")</formula>
+      <formula>(H6="XX ")OR (H6="OO ")OR (H6="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
@@ -2632,7 +2683,7 @@
       <formula>(H7="")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="252">
-      <formula>(H7="XX")OR (H7="OO")OR (H7="TT")</formula>
+      <formula>(H7="XX ")OR (H7="OO ")OR (H7="TT ")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>